<commit_message>
lectura de datos desde json
</commit_message>
<xml_diff>
--- a/Seguimiento-Consignas/Cumplimiento-Consignas.xlsx
+++ b/Seguimiento-Consignas/Cumplimiento-Consignas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Cusro-CodoACodo\03-PythonFS-24172\C24172G11\Seguimiento-Consignas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C187C018-007A-40A4-9C6D-301346285591}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE592AEC-F091-40E6-93DB-64392279D8B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="345" yWindow="0" windowWidth="20145" windowHeight="11520" xr2:uid="{E73603EF-647A-4F8D-8F20-EFE93E8FD641}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
   <si>
     <t>Utilizar al menos una animación, transformación o una transición.</t>
   </si>
@@ -127,6 +127,9 @@
   </si>
   <si>
     <t xml:space="preserve">SLC: se utilizo Flexbox y responsive en todas las paginas. </t>
+  </si>
+  <si>
+    <t>SLC: la pagina catalogo pasa a la pagina catitems la categoria. La pagina catitems se arma con una api que lee los articulos pertenecientes a la categoria desd un archivo json</t>
   </si>
 </sst>
 </file>
@@ -203,7 +206,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -228,6 +231,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -566,8 +572,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD66D113-014E-4A55-AA96-4F35F8EF79FF}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -641,6 +647,12 @@
       <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
+      <c r="B7" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="8" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">

</xml_diff>

<commit_message>
2024-05-01: cambios varios para antesResponsive
</commit_message>
<xml_diff>
--- a/Seguimiento-Consignas/Cumplimiento-Consignas.xlsx
+++ b/Seguimiento-Consignas/Cumplimiento-Consignas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Cusro-CodoACodo\03-PythonFS-24172\C24172G11\Seguimiento-Consignas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE592AEC-F091-40E6-93DB-64392279D8B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA6BA8C0-DB61-4A47-9FD0-5E5AEC743D52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="345" yWindow="0" windowWidth="20145" windowHeight="11520" xr2:uid="{E73603EF-647A-4F8D-8F20-EFE93E8FD641}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{E73603EF-647A-4F8D-8F20-EFE93E8FD641}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="26">
   <si>
     <t>Utilizar al menos una animación, transformación o una transición.</t>
   </si>
@@ -102,34 +102,49 @@
     <t>SI</t>
   </si>
   <si>
-    <t>SLC: si bien esta en revision la decision del formato final superamos las 4 pagias</t>
-  </si>
-  <si>
     <t>En progreso</t>
   </si>
   <si>
     <t>https://github.com/contesl/C24172G11</t>
   </si>
   <si>
-    <t>SLC: cuando finalizamos ahí la podemos subir sin problemas</t>
-  </si>
-  <si>
-    <t>SLC: el sitio utiliza etiquetas semánticas</t>
-  </si>
-  <si>
-    <t>SLC: si bien esta en revision la decision del formato final el sitio utiliza iFrame en la pagina Who is</t>
-  </si>
-  <si>
-    <t>SLC: se utiliza una transicion en las imagines de catalog.html. Hay que revisar el efecto</t>
-  </si>
-  <si>
-    <t>SLC: hay un formulario "enganchado" pero tomando el que hizo el profe en clase. Hay que reprogramarlo completo y agregar validaciones javascript (yo tengo ejemplos)- La validaciones javascript hay que ponerlas en el archivo externo contenido en /js</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SLC: se utilizo Flexbox y responsive en todas las paginas. </t>
-  </si>
-  <si>
-    <t>SLC: la pagina catalogo pasa a la pagina catitems la categoria. La pagina catitems se arma con una api que lee los articulos pertenecientes a la categoria desd un archivo json</t>
+    <t>La pagina catalogo.html pasa a la pagina catitems.html el valor de  la categoria seleccionada.
+ La pagina catitems.html se genera en forma dinamica con una api que lee los articulos pertenecientes a la categoria desde un archivo JSON existente en disco.</t>
+  </si>
+  <si>
+    <t>El sitio utiliza etiquetas semánticas</t>
+  </si>
+  <si>
+    <t>Ell sitio utiliza iFrame en la pagina Who is (whois.html)</t>
+  </si>
+  <si>
+    <t>El sitio completo tiene 7 paginas
+index.html = pagina principal
+whatis.html = explica que es SportsPro
+whois.html = explica quienes somos y la localizacion geografica
+catalog.html = para elegir una categoria del catalogo de articulos
+catiitems.html = presenta los articulos de una categoria y permite realizar el pedido
+order.html = permite completar la compra ingresando datos de envio y pago (CRUD)
+contacto.html = permite dejar los datos de contacto (CRUD)</t>
+  </si>
+  <si>
+    <t>Se cumple con la pagina contacto.html</t>
+  </si>
+  <si>
+    <t>Todas las paginas del sitio son responsive con 3 puntos de corte
+media only screen and (max-width: 320px)
+media only screen and (max-width: 720px)
+media only screen and (min-width: 1025px)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se utiliza una animacion/transicion en las imagines de catalog.html. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se utilizo Flexbox y Grid en todas las paginas
+</t>
+  </si>
+  <si>
+    <t>Cuando finalizamos ahí la podemos subir sin problemas</t>
   </si>
 </sst>
 </file>
@@ -206,7 +221,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -233,6 +248,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -572,8 +590,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD66D113-014E-4A55-AA96-4F35F8EF79FF}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -594,31 +612,37 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="120" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>15</v>
+      <c r="C2" s="9" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>16</v>
+      <c r="B3" s="7" t="s">
+        <v>14</v>
       </c>
       <c r="C3" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="9" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -629,29 +653,29 @@
         <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
         <v>1</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C6" t="s">
-        <v>23</v>
+      <c r="C6" s="3" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>16</v>
+      <c r="B7" s="7" t="s">
+        <v>14</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="60" x14ac:dyDescent="0.25">
@@ -667,7 +691,7 @@
         <v>14</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="45" x14ac:dyDescent="0.25">
@@ -675,10 +699,10 @@
         <v>11</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="45" x14ac:dyDescent="0.25">
@@ -689,7 +713,7 @@
         <v>14</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="45" x14ac:dyDescent="0.25">
@@ -700,7 +724,7 @@
         <v>14</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualizacion de la planilla de control control el nombre de la subida al site
</commit_message>
<xml_diff>
--- a/Seguimiento-Consignas/Cumplimiento-Consignas.xlsx
+++ b/Seguimiento-Consignas/Cumplimiento-Consignas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Cusro-CodoACodo\03-PythonFS-24172\C24172G11\Seguimiento-Consignas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA6BA8C0-DB61-4A47-9FD0-5E5AEC743D52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27DDBD2E-3202-4C18-96F8-8A6B6C15D70A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{E73603EF-647A-4F8D-8F20-EFE93E8FD641}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
   <si>
     <t>Utilizar al menos una animación, transformación o una transición.</t>
   </si>
@@ -100,9 +100,6 @@
   </si>
   <si>
     <t>SI</t>
-  </si>
-  <si>
-    <t>En progreso</t>
   </si>
   <si>
     <t>https://github.com/contesl/C24172G11</t>
@@ -144,7 +141,7 @@
 </t>
   </si>
   <si>
-    <t>Cuando finalizamos ahí la podemos subir sin problemas</t>
+    <t>https://sportspro.netlify.app/</t>
   </si>
 </sst>
 </file>
@@ -176,18 +173,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -226,22 +217,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
@@ -250,8 +238,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -590,8 +581,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD66D113-014E-4A55-AA96-4F35F8EF79FF}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -616,66 +607,66 @@
       <c r="A2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>20</v>
+      <c r="B2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="6" t="s">
+      <c r="B3" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="8" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="6" t="s">
         <v>14</v>
       </c>
       <c r="C5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>17</v>
+      <c r="B7" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="60" x14ac:dyDescent="0.25">
@@ -687,49 +678,50 @@
       <c r="A9" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>16</v>
+      <c r="B9" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>25</v>
+      <c r="B10" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="6" t="s">
         <v>14</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="6" t="s">
         <v>14</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C9" r:id="rId1" xr:uid="{E68218D7-7F14-4D5F-AAEB-EBAA80884284}"/>
+    <hyperlink ref="C10" r:id="rId2" xr:uid="{B17DF635-5D67-4C69-B432-9341559C1C1E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
modificacion en el link del site
</commit_message>
<xml_diff>
--- a/Seguimiento-Consignas/Cumplimiento-Consignas.xlsx
+++ b/Seguimiento-Consignas/Cumplimiento-Consignas.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Cusro-CodoACodo\03-PythonFS-24172\C24172G11\Seguimiento-Consignas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27DDBD2E-3202-4C18-96F8-8A6B6C15D70A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD096298-63EB-4B33-B757-A7C5760D7720}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{E73603EF-647A-4F8D-8F20-EFE93E8FD641}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="24">
   <si>
     <t>Utilizar al menos una animación, transformación o una transición.</t>
   </si>
@@ -139,9 +139,6 @@
   <si>
     <t xml:space="preserve">Se utilizo Flexbox y Grid en todas las paginas
 </t>
-  </si>
-  <si>
-    <t>https://sportspro.netlify.app/</t>
   </si>
 </sst>
 </file>
@@ -582,7 +579,7 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -693,7 +690,7 @@
         <v>14</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="45" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
cambio en el link de la pagina
</commit_message>
<xml_diff>
--- a/Seguimiento-Consignas/Cumplimiento-Consignas.xlsx
+++ b/Seguimiento-Consignas/Cumplimiento-Consignas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Cusro-CodoACodo\03-PythonFS-24172\C24172G11\Seguimiento-Consignas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\C24172G11\Seguimiento-Consignas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD096298-63EB-4B33-B757-A7C5760D7720}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6FAF6C4-633E-4623-AB77-4F0E8D0AFA21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{E73603EF-647A-4F8D-8F20-EFE93E8FD641}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{E73603EF-647A-4F8D-8F20-EFE93E8FD641}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
   <si>
     <t>Utilizar al menos una animación, transformación o una transición.</t>
   </si>
@@ -139,6 +139,9 @@
   <si>
     <t xml:space="preserve">Se utilizo Flexbox y Grid en todas las paginas
 </t>
+  </si>
+  <si>
+    <t>https://contesl.github.io/C24172G11/</t>
   </si>
 </sst>
 </file>
@@ -578,18 +581,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD66D113-014E-4A55-AA96-4F35F8EF79FF}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B6" workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="68.28515625" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" customWidth="1"/>
-    <col min="3" max="3" width="98.140625" customWidth="1"/>
+    <col min="1" max="1" width="68.26953125" customWidth="1"/>
+    <col min="2" max="2" width="13.7265625" customWidth="1"/>
+    <col min="3" max="3" width="98.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -600,7 +603,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="120" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="116" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>6</v>
       </c>
@@ -611,7 +614,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="58" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -622,7 +625,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="58" x14ac:dyDescent="0.35">
       <c r="A4" s="9" t="s">
         <v>7</v>
       </c>
@@ -633,7 +636,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>0</v>
       </c>
@@ -644,7 +647,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A6" s="9" t="s">
         <v>1</v>
       </c>
@@ -655,7 +658,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
@@ -666,12 +669,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="58" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>9</v>
       </c>
@@ -682,7 +685,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
         <v>11</v>
       </c>
@@ -690,10 +693,10 @@
         <v>14</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>12</v>
       </c>
@@ -704,7 +707,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
         <v>13</v>
       </c>

</xml_diff>